<commit_message>
Updated "INFO Analysis" tab with the new platform CVs
</commit_message>
<xml_diff>
--- a/src/files/EVA_Submission_template.V1.1.3.xlsx
+++ b/src/files/EVA_Submission_template.V1.1.3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="993" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="993" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="12" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="539">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2381,6 +2381,27 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2391,27 +2412,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2875,8 +2875,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1">
-      <c r="A1" s="76"/>
-      <c r="B1" s="76"/>
+      <c r="A1" s="83"/>
+      <c r="B1" s="83"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -2885,10 +2885,10 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="26.25">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="77"/>
+      <c r="B2" s="84"/>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
       <c r="E2" s="51"/>
@@ -2897,8 +2897,8 @@
       <c r="H2" s="51"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="18.75">
-      <c r="A3" s="78"/>
-      <c r="B3" s="78"/>
+      <c r="A3" s="85"/>
+      <c r="B3" s="85"/>
       <c r="C3" s="52"/>
       <c r="D3" s="52"/>
       <c r="E3" s="52"/>
@@ -2919,8 +2919,8 @@
       <c r="H4" s="53"/>
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80"/>
+      <c r="A5" s="78"/>
+      <c r="B5" s="78"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -2941,10 +2941,10 @@
       <c r="H6" s="53"/>
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" ht="18.75">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="75"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="54"/>
       <c r="D7" s="54"/>
       <c r="E7" s="54"/>
@@ -2953,8 +2953,8 @@
       <c r="H7" s="54"/>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1">
-      <c r="A8" s="83"/>
-      <c r="B8" s="80"/>
+      <c r="A8" s="77"/>
+      <c r="B8" s="78"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -2975,8 +2975,8 @@
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1">
-      <c r="A10" s="80"/>
-      <c r="B10" s="80"/>
+      <c r="A10" s="78"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -2985,10 +2985,10 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" s="29" customFormat="1" ht="19.5" thickBot="1">
-      <c r="A11" s="84" t="s">
+      <c r="A11" s="80" t="s">
         <v>521</v>
       </c>
-      <c r="B11" s="84"/>
+      <c r="B11" s="80"/>
     </row>
     <row r="12" spans="1:8" s="29" customFormat="1" ht="18.75">
       <c r="A12" s="55" t="s">
@@ -3041,28 +3041,28 @@
     </row>
     <row r="18" spans="1:2" s="29" customFormat="1"/>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="85" t="s">
+      <c r="A19" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="85"/>
+      <c r="B19" s="81"/>
     </row>
     <row r="20" spans="1:2" ht="18.75">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="75" t="s">
         <v>524</v>
       </c>
-      <c r="B20" s="81"/>
+      <c r="B20" s="75"/>
     </row>
     <row r="21" spans="1:2" ht="18.75">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="81"/>
+      <c r="B21" s="75"/>
     </row>
     <row r="22" spans="1:2" ht="18.75">
-      <c r="A22" s="82" t="s">
+      <c r="A22" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="82"/>
+      <c r="B22" s="76"/>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1">
       <c r="A23" s="63" t="s">
@@ -3129,6 +3129,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A8:B8"/>
@@ -3137,12 +3143,6 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3194,8 +3194,8 @@
   </sheetPr>
   <dimension ref="A1:L281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -6307,10 +6307,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -6461,128 +6461,168 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>182</v>
+      <c r="A22" s="12" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>183</v>
+        <v>536</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>184</v>
+        <v>535</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>531</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>186</v>
+      <c r="A26" s="12" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>531</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>205</v>
+        <v>538</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
         <v>206</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>